<commit_message>
Experiments update for master data
</commit_message>
<xml_diff>
--- a/Experiments/DetectEvent/data/p06_visual_pick_gougeevents_merged.xlsx
+++ b/Experiments/DetectEvent/data/p06_visual_pick_gougeevents_merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kokubo/Dropbox/NIED_RESEARCH/4mBIAX_submission/4mNonSelfSim_Paper/Experiments/DetectEvent/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC85D32C-A820-B245-B7D6-75CE8770EE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F49414-7B18-6344-8A86-C484A4F15599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2920" windowWidth="28740" windowHeight="21160" xr2:uid="{CAF4AC9E-8B8C-5842-900A-3EB882FF1CD6}"/>
+    <workbookView xWindow="3240" yWindow="3080" windowWidth="28740" windowHeight="21160" xr2:uid="{CAF4AC9E-8B8C-5842-900A-3EB882FF1CD6}"/>
   </bookViews>
   <sheets>
     <sheet name="p06_visual_pick_gougeevents_mer" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t># This pick time is a crude estimation using p06_search_gougeevents.m. We need to relocate the hypocenter and event origin time from the picks listed below.</t>
-  </si>
-  <si>
-    <t># expr_id: index of experiments, event_id: index of stick-slip main events, gouge_loc [m]: location of gouge patch,  picktime [s]: event time of seismic event, AEtype: Ordinary or LFE, rup_type: nucleation location</t>
   </si>
   <si>
     <t>expr_id</t>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>old_gougeevent_id</t>
+  </si>
+  <si>
+    <t># expr_id: index of experiments, event_id: index of stick-slip main events, gouge_loc [m]: location of gouge patch,  picktime [s]: event time of seismic event, eventtype: Ordinary or LFE, rup_type: nucleation location</t>
   </si>
 </sst>
 </file>
@@ -928,7 +928,7 @@
   <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,41 +945,41 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -991,7 +991,7 @@
         <v>41.024999999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1020,7 +1020,7 @@
         <v>42.463999999999999</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1049,7 +1049,7 @@
         <v>42.464500000000001</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1066,7 +1066,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1078,7 +1078,7 @@
         <v>42.4679</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1107,7 +1107,7 @@
         <v>42.47475</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -1136,7 +1136,7 @@
         <v>43.623150000000003</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1165,7 +1165,7 @@
         <v>43.624000000000002</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1194,7 +1194,7 @@
         <v>43.625399999999999</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -1223,7 +1223,7 @@
         <v>47.658000000000001</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -1252,7 +1252,7 @@
         <v>47.662700000000001</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1281,7 +1281,7 @@
         <v>47.663899999999998</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -1310,7 +1310,7 @@
         <v>47.664549999999998</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -1339,7 +1339,7 @@
         <v>49.178100000000001</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>6</v>
@@ -1368,7 +1368,7 @@
         <v>49.182200000000002</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -1397,7 +1397,7 @@
         <v>49.1828</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1426,7 +1426,7 @@
         <v>49.185899999999997</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1455,7 +1455,7 @@
         <v>54.525350000000003</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>7</v>
@@ -1484,7 +1484,7 @@
         <v>54.543399999999998</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -1513,7 +1513,7 @@
         <v>56.726999999999997</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -1542,7 +1542,7 @@
         <v>59.103149999999999</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1559,7 +1559,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>9</v>
@@ -1571,7 +1571,7 @@
         <v>59.103499999999997</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -1600,7 +1600,7 @@
         <v>63.752299999999998</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -1629,7 +1629,7 @@
         <v>63.756999999999998</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>10</v>
@@ -1658,7 +1658,7 @@
         <v>63.757899999999999</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29">
         <v>2</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>11</v>
@@ -1687,7 +1687,7 @@
         <v>66.186899999999994</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>12</v>
@@ -1716,7 +1716,7 @@
         <v>68.488100000000003</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>12</v>
@@ -1745,7 +1745,7 @@
         <v>68.489900000000006</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>14</v>
@@ -1774,7 +1774,7 @@
         <v>76.0184</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>14</v>
@@ -1803,7 +1803,7 @@
         <v>76.023499999999999</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35">
         <v>15</v>
@@ -1832,7 +1832,7 @@
         <v>79.316699999999997</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35">
         <v>3</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>15</v>
@@ -1861,7 +1861,7 @@
         <v>79.319850000000002</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36">
         <v>3</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>15</v>
@@ -1890,7 +1890,7 @@
         <v>79.320099999999996</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37">
         <v>3</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>15</v>
@@ -1919,7 +1919,7 @@
         <v>79.325400000000002</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38">
         <v>3</v>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>15</v>
@@ -1948,7 +1948,7 @@
         <v>79.333399999999997</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>16</v>
@@ -1977,7 +1977,7 @@
         <v>82.286100000000005</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>17</v>
@@ -2006,7 +2006,7 @@
         <v>85.981099999999998</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>17</v>
@@ -2035,7 +2035,7 @@
         <v>85.985900000000001</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>17</v>
@@ -2064,7 +2064,7 @@
         <v>85.987449999999995</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2081,7 +2081,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
         <v>17</v>
@@ -2093,7 +2093,7 @@
         <v>85.988500000000002</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>17</v>
@@ -2122,7 +2122,7 @@
         <v>85.989099999999993</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
         <v>18</v>
@@ -2151,7 +2151,7 @@
         <v>91.300700000000006</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>18</v>
@@ -2180,7 +2180,7 @@
         <v>91.302300000000002</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48">
         <v>18</v>
@@ -2209,7 +2209,7 @@
         <v>91.303100000000001</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
         <v>18</v>
@@ -2238,7 +2238,7 @@
         <v>91.311000000000007</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50">
         <v>19</v>
@@ -2267,7 +2267,7 @@
         <v>94.407340000000005</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F50">
         <v>3</v>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B51">
         <v>19</v>
@@ -2296,7 +2296,7 @@
         <v>94.407449999999997</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51">
         <v>3</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B52">
         <v>19</v>
@@ -2325,7 +2325,7 @@
         <v>94.418800000000005</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52">
         <v>3</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53">
         <v>20</v>
@@ -2354,7 +2354,7 @@
         <v>97.360399999999998</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54">
         <v>21</v>
@@ -2383,7 +2383,7 @@
         <v>100.5903</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -2400,7 +2400,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55">
         <v>21</v>
@@ -2412,7 +2412,7 @@
         <v>100.59555</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F55">
         <v>3</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B56">
         <v>21</v>
@@ -2441,7 +2441,7 @@
         <v>100.5958</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F56">
         <v>3</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57">
         <v>21</v>
@@ -2470,7 +2470,7 @@
         <v>100.6006</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58">
         <v>21</v>
@@ -2499,7 +2499,7 @@
         <v>100.60335000000001</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F58">
         <v>3</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B59">
         <v>22</v>
@@ -2528,7 +2528,7 @@
         <v>105.9759</v>
       </c>
       <c r="E59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60">
         <v>23</v>
@@ -2557,7 +2557,7 @@
         <v>108.95140000000001</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F60">
         <v>3</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>23</v>
@@ -2586,7 +2586,7 @@
         <v>108.9568</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F61">
         <v>3</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B62">
         <v>23</v>
@@ -2615,7 +2615,7 @@
         <v>108.95829999999999</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F62">
         <v>3</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B63">
         <v>23</v>
@@ -2644,7 +2644,7 @@
         <v>108.96120000000001</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F63">
         <v>3</v>
@@ -2661,7 +2661,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B64">
         <v>24</v>
@@ -2673,7 +2673,7 @@
         <v>111.8541</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F64">
         <v>2</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B65">
         <v>25</v>
@@ -2702,7 +2702,7 @@
         <v>116.23725</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66">
         <v>25</v>
@@ -2731,7 +2731,7 @@
         <v>116.23860000000001</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67">
         <v>25</v>
@@ -2760,7 +2760,7 @@
         <v>116.2403</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B68">
         <v>26</v>
@@ -2789,7 +2789,7 @@
         <v>120.77835</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B69">
         <v>26</v>
@@ -2818,7 +2818,7 @@
         <v>120.7843</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B70">
         <v>27</v>
@@ -2847,7 +2847,7 @@
         <v>123.88305</v>
       </c>
       <c r="E70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2864,7 +2864,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71">
         <v>27</v>
@@ -2876,7 +2876,7 @@
         <v>123.8879</v>
       </c>
       <c r="E71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2893,7 +2893,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72">
         <v>27</v>
@@ -2905,7 +2905,7 @@
         <v>123.8888</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B73">
         <v>27</v>
@@ -2934,7 +2934,7 @@
         <v>123.9008</v>
       </c>
       <c r="E73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74">
         <v>27</v>
@@ -2963,7 +2963,7 @@
         <v>123.90585</v>
       </c>
       <c r="E74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B75">
         <v>27</v>
@@ -2992,7 +2992,7 @@
         <v>123.9217</v>
       </c>
       <c r="E75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -3009,7 +3009,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B76">
         <v>28</v>
@@ -3021,7 +3021,7 @@
         <v>126.8502</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F76">
         <v>2</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B77">
         <v>29</v>
@@ -3050,7 +3050,7 @@
         <v>130.72714999999999</v>
       </c>
       <c r="E77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B78">
         <v>29</v>
@@ -3079,7 +3079,7 @@
         <v>130.7345</v>
       </c>
       <c r="E78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B79">
         <v>30</v>
@@ -3108,7 +3108,7 @@
         <v>135.41040000000001</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F79">
         <v>2</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B80">
         <v>30</v>
@@ -3137,7 +3137,7 @@
         <v>135.41229999999999</v>
       </c>
       <c r="E80" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F80">
         <v>2</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B81">
         <v>31</v>
@@ -3166,7 +3166,7 @@
         <v>138.54830000000001</v>
       </c>
       <c r="E81" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F81">
         <v>3</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B82">
         <v>31</v>
@@ -3195,7 +3195,7 @@
         <v>138.54949999999999</v>
       </c>
       <c r="E82" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F82">
         <v>3</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B83">
         <v>31</v>
@@ -3224,7 +3224,7 @@
         <v>138.55080000000001</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F83">
         <v>3</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B84">
         <v>32</v>
@@ -3253,7 +3253,7 @@
         <v>142.04839999999999</v>
       </c>
       <c r="E84" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F84">
         <v>2</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B85">
         <v>32</v>
@@ -3282,7 +3282,7 @@
         <v>142.0548</v>
       </c>
       <c r="E85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F85">
         <v>2</v>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B86">
         <v>32</v>
@@ -3311,7 +3311,7 @@
         <v>142.06585000000001</v>
       </c>
       <c r="E86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F86">
         <v>2</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B87">
         <v>33</v>
@@ -3340,7 +3340,7 @@
         <v>146.5368</v>
       </c>
       <c r="E87" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B88">
         <v>33</v>
@@ -3369,7 +3369,7 @@
         <v>146.5386</v>
       </c>
       <c r="E88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B89">
         <v>33</v>
@@ -3398,7 +3398,7 @@
         <v>146.54075</v>
       </c>
       <c r="E89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B90">
         <v>34</v>
@@ -3427,7 +3427,7 @@
         <v>151.69225</v>
       </c>
       <c r="E90" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F90">
         <v>2</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B91">
         <v>34</v>
@@ -3456,7 +3456,7 @@
         <v>151.69919999999999</v>
       </c>
       <c r="E91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F91">
         <v>2</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B92">
         <v>34</v>
@@ -3485,7 +3485,7 @@
         <v>151.70310000000001</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F92">
         <v>2</v>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B93">
         <v>34</v>
@@ -3514,7 +3514,7 @@
         <v>151.72020000000001</v>
       </c>
       <c r="E93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F93">
         <v>2</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B94">
         <v>35</v>
@@ -3543,7 +3543,7 @@
         <v>161.09719999999999</v>
       </c>
       <c r="E94" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F94">
         <v>3</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B95">
         <v>35</v>
@@ -3572,7 +3572,7 @@
         <v>161.12010000000001</v>
       </c>
       <c r="E95" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B96">
         <v>35</v>
@@ -3601,7 +3601,7 @@
         <v>161.12755000000001</v>
       </c>
       <c r="E96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F96">
         <v>3</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B97">
         <v>36</v>
@@ -3630,7 +3630,7 @@
         <v>164.10480000000001</v>
       </c>
       <c r="E97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F97">
         <v>2</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B98">
         <v>36</v>
@@ -3659,7 +3659,7 @@
         <v>164.10990000000001</v>
       </c>
       <c r="E98" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F98">
         <v>2</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B99">
         <v>36</v>
@@ -3688,7 +3688,7 @@
         <v>164.11840000000001</v>
       </c>
       <c r="E99" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F99">
         <v>2</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B100">
         <v>37</v>
@@ -3717,7 +3717,7 @@
         <v>167.28569999999999</v>
       </c>
       <c r="E100" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3734,7 +3734,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B101">
         <v>37</v>
@@ -3746,7 +3746,7 @@
         <v>167.2868</v>
       </c>
       <c r="E101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -3763,7 +3763,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B102">
         <v>38</v>
@@ -3775,7 +3775,7 @@
         <v>172.2182</v>
       </c>
       <c r="E102" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F102">
         <v>2</v>
@@ -3792,7 +3792,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B103">
         <v>38</v>
@@ -3804,7 +3804,7 @@
         <v>172.24029999999999</v>
       </c>
       <c r="E103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F103">
         <v>2</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B104">
         <v>39</v>
@@ -3833,7 +3833,7 @@
         <v>175.3845</v>
       </c>
       <c r="E104" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F104">
         <v>3</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B105">
         <v>39</v>
@@ -3862,7 +3862,7 @@
         <v>175.38550000000001</v>
       </c>
       <c r="E105" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F105">
         <v>3</v>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B106">
         <v>39</v>
@@ -3891,7 +3891,7 @@
         <v>175.39109999999999</v>
       </c>
       <c r="E106" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F106">
         <v>3</v>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B107">
         <v>40</v>
@@ -3920,7 +3920,7 @@
         <v>178.94640000000001</v>
       </c>
       <c r="E107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F107">
         <v>2</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B108">
         <v>40</v>
@@ -3949,7 +3949,7 @@
         <v>178.9546</v>
       </c>
       <c r="E108" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F108">
         <v>2</v>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B109">
         <v>41</v>
@@ -3978,7 +3978,7 @@
         <v>186.2612</v>
       </c>
       <c r="E109" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F109">
         <v>3</v>
@@ -3995,7 +3995,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B110">
         <v>41</v>
@@ -4007,7 +4007,7 @@
         <v>186.26310000000001</v>
       </c>
       <c r="E110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F110">
         <v>3</v>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B111">
         <v>41</v>
@@ -4036,7 +4036,7 @@
         <v>186.2679</v>
       </c>
       <c r="E111" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F111">
         <v>3</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B112">
         <v>41</v>
@@ -4065,7 +4065,7 @@
         <v>186.28</v>
       </c>
       <c r="E112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F112">
         <v>3</v>
@@ -4082,7 +4082,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B113">
         <v>41</v>
@@ -4094,7 +4094,7 @@
         <v>186.28614999999999</v>
       </c>
       <c r="E113" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F113">
         <v>3</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B114">
         <v>41</v>
@@ -4123,7 +4123,7 @@
         <v>186.2869</v>
       </c>
       <c r="E114" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F114">
         <v>3</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B115">
         <v>42</v>
@@ -4152,7 +4152,7 @@
         <v>190.16040000000001</v>
       </c>
       <c r="E115" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F115">
         <v>2</v>
@@ -4169,7 +4169,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B116">
         <v>43</v>
@@ -4181,7 +4181,7 @@
         <v>193.77199999999999</v>
       </c>
       <c r="E116" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -4198,7 +4198,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B117">
         <v>43</v>
@@ -4210,7 +4210,7 @@
         <v>193.7842</v>
       </c>
       <c r="E117" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B118">
         <v>44</v>
@@ -4239,7 +4239,7 @@
         <v>197.62190000000001</v>
       </c>
       <c r="E118" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B119">
         <v>44</v>
@@ -4268,7 +4268,7 @@
         <v>197.62440000000001</v>
       </c>
       <c r="E119" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F119">
         <v>2</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B120">
         <v>44</v>
@@ -4297,7 +4297,7 @@
         <v>197.63249999999999</v>
       </c>
       <c r="E120" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F120">
         <v>2</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B121">
         <v>45</v>
@@ -4326,7 +4326,7 @@
         <v>207.42904999999999</v>
       </c>
       <c r="E121" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -4343,7 +4343,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B122">
         <v>45</v>
@@ -4355,7 +4355,7 @@
         <v>207.46090000000001</v>
       </c>
       <c r="E122" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -4372,7 +4372,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B123">
         <v>46</v>
@@ -4384,7 +4384,7 @@
         <v>211.09110000000001</v>
       </c>
       <c r="E123" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F123">
         <v>2</v>
@@ -4401,7 +4401,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B124">
         <v>46</v>
@@ -4413,7 +4413,7 @@
         <v>211.10239999999999</v>
       </c>
       <c r="E124" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F124">
         <v>2</v>
@@ -4430,7 +4430,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B125">
         <v>48</v>
@@ -4442,7 +4442,7 @@
         <v>220.2576</v>
       </c>
       <c r="E125" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F125">
         <v>2</v>
@@ -4459,7 +4459,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B126">
         <v>49</v>
@@ -4471,7 +4471,7 @@
         <v>225.89070000000001</v>
       </c>
       <c r="E126" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B127">
         <v>50</v>
@@ -4500,7 +4500,7 @@
         <v>228.7646</v>
       </c>
       <c r="E127" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F127">
         <v>2</v>
@@ -4517,7 +4517,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B128">
         <v>50</v>
@@ -4529,7 +4529,7 @@
         <v>228.78745000000001</v>
       </c>
       <c r="E128" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F128">
         <v>2</v>
@@ -4546,7 +4546,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B129">
         <v>51</v>
@@ -4558,7 +4558,7 @@
         <v>232.20574999999999</v>
       </c>
       <c r="E129" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B130">
         <v>51</v>
@@ -4587,7 +4587,7 @@
         <v>232.21209999999999</v>
       </c>
       <c r="E130" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B131">
         <v>52</v>
@@ -4616,7 +4616,7 @@
         <v>235.63079999999999</v>
       </c>
       <c r="E131" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F131">
         <v>2</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B132">
         <v>52</v>
@@ -4645,7 +4645,7 @@
         <v>235.63149999999999</v>
       </c>
       <c r="E132" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F132">
         <v>2</v>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B133">
         <v>53</v>
@@ -4674,7 +4674,7 @@
         <v>241.46700000000001</v>
       </c>
       <c r="E133" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F133">
         <v>1</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B134">
         <v>53</v>
@@ -4703,7 +4703,7 @@
         <v>241.5129</v>
       </c>
       <c r="E134" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F134">
         <v>1</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B135">
         <v>54</v>
@@ -4732,7 +4732,7 @@
         <v>245.07105000000001</v>
       </c>
       <c r="E135" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F135">
         <v>2</v>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B136">
         <v>54</v>
@@ -4761,7 +4761,7 @@
         <v>245.07470000000001</v>
       </c>
       <c r="E136" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F136">
         <v>2</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B137">
         <v>55</v>
@@ -4790,7 +4790,7 @@
         <v>248.90199999999999</v>
       </c>
       <c r="E137" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F137">
         <v>1</v>
@@ -4807,7 +4807,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B138">
         <v>55</v>
@@ -4819,7 +4819,7 @@
         <v>248.90809999999999</v>
       </c>
       <c r="E138" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F138">
         <v>1</v>

</xml_diff>